<commit_message>
add bitwise transpose function
</commit_message>
<xml_diff>
--- a/solutions/small_nonogram_solver.xlsx
+++ b/solutions/small_nonogram_solver.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H155936\Documents\GitHub\codewars\solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485F9E55-D191-4061-B581-9194CA94F161}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -146,6 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,11 +461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,12 +473,12 @@
     <col min="2" max="6" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -484,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -501,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -514,9 +516,14 @@
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>0</v>
       </c>
@@ -529,9 +536,14 @@
       <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>0</v>
       </c>
@@ -544,9 +556,14 @@
       <c r="E7" s="10">
         <v>1</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>0</v>
       </c>
@@ -559,9 +576,14 @@
       <c r="E8" s="10">
         <v>0</v>
       </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>0</v>
       </c>
@@ -574,7 +596,32 @@
       <c r="E9" s="8">
         <v>0</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add function to set known zeros.
</commit_message>
<xml_diff>
--- a/solutions/small_nonogram_solver.xlsx
+++ b/solutions/small_nonogram_solver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H155936\Documents\GitHub\codewars\solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C6D6AB-F116-4B29-A799-CF16CE1E8686}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E14FD6-50B9-4F14-B73E-73ED964D182D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14424" windowHeight="6804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>2, 1</t>
   </si>
@@ -51,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -139,11 +139,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -158,6 +195,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,23 +512,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="6" width="3.109375" customWidth="1"/>
+    <col min="9" max="13" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -496,7 +537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -513,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -532,8 +573,9 @@
       <c r="G5" s="10">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>0</v>
       </c>
@@ -552,8 +594,9 @@
       <c r="G6" s="10">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>0</v>
       </c>
@@ -572,8 +615,9 @@
       <c r="G7" s="10">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>0</v>
       </c>
@@ -592,8 +636,9 @@
       <c r="G8" s="10">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>0</v>
       </c>
@@ -612,8 +657,9 @@
       <c r="G9" s="10">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="10">
         <v>0</v>
       </c>
@@ -630,10 +676,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -653,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -673,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -693,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
@@ -713,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -732,6 +778,187 @@
       <c r="F17" s="9">
         <v>0</v>
       </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="12">
+        <v>1</v>
+      </c>
+      <c r="J23" s="13">
+        <v>1</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="13">
+        <v>1</v>
+      </c>
+      <c r="K24" s="13">
+        <v>1</v>
+      </c>
+      <c r="L24" s="13"/>
+      <c r="M24" s="14"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13">
+        <v>1</v>
+      </c>
+      <c r="L25" s="13">
+        <v>1</v>
+      </c>
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13">
+        <v>1</v>
+      </c>
+      <c r="M26" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
In progress: find next variants when a set of '0's and '1's has been found.
</commit_message>
<xml_diff>
--- a/solutions/small_nonogram_solver.xlsx
+++ b/solutions/small_nonogram_solver.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H155936\Documents\GitHub\codewars\solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E14FD6-50B9-4F14-B73E-73ED964D182D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587ACA3-ACFF-45F9-B910-C07E7EB7DDDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14424" windowHeight="6804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -514,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,6 +743,10 @@
       <c r="F15" s="6">
         <v>0</v>
       </c>
+      <c r="H15">
+        <f>(50+50)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">

</xml_diff>

<commit_message>
In progress: build combinator generator that issues all possible combinations of "0"s and "1"s for a given tuple of clues (either for a row or column).
</commit_message>
<xml_diff>
--- a/solutions/small_nonogram_solver.xlsx
+++ b/solutions/small_nonogram_solver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H155936\Documents\GitHub\codewars\solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587ACA3-ACFF-45F9-B910-C07E7EB7DDDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF9E5C4-BE3D-4B29-9E30-812403DB1A4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14424" windowHeight="6804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,24 +517,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M27"/>
+  <dimension ref="A2:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AM32" sqref="AM32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="3.109375" customWidth="1"/>
-    <col min="9" max="13" width="3" customWidth="1"/>
+    <col min="2" max="6" width="3.140625" customWidth="1"/>
+    <col min="9" max="27" width="3.140625" customWidth="1"/>
+    <col min="28" max="38" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -542,7 +543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -559,7 +560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -580,7 +581,7 @@
       </c>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>0</v>
       </c>
@@ -601,7 +602,7 @@
       </c>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>0</v>
       </c>
@@ -622,7 +623,7 @@
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>0</v>
       </c>
@@ -643,7 +644,7 @@
       </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>0</v>
       </c>
@@ -664,7 +665,7 @@
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>0</v>
       </c>
@@ -681,10 +682,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -704,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -724,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -748,7 +749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
@@ -768,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -788,26 +789,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1</v>
       </c>
@@ -815,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1</v>
       </c>
@@ -832,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -864,7 +865,7 @@
       <c r="L23" s="13"/>
       <c r="M23" s="14"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -890,7 +891,7 @@
       <c r="L24" s="13"/>
       <c r="M24" s="14"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -922,7 +923,7 @@
       </c>
       <c r="M25" s="14"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>0</v>
       </c>
@@ -948,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -969,6 +970,279 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
     </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>5</v>
+      </c>
+      <c r="N28">
+        <v>6</v>
+      </c>
+      <c r="O28">
+        <v>7</v>
+      </c>
+      <c r="P28">
+        <v>8</v>
+      </c>
+      <c r="Q28">
+        <v>9</v>
+      </c>
+      <c r="R28">
+        <v>10</v>
+      </c>
+      <c r="S28">
+        <v>11</v>
+      </c>
+      <c r="T28">
+        <v>12</v>
+      </c>
+      <c r="U28">
+        <v>13</v>
+      </c>
+      <c r="V28">
+        <v>14</v>
+      </c>
+      <c r="W28">
+        <v>15</v>
+      </c>
+      <c r="X28">
+        <v>16</v>
+      </c>
+      <c r="Y28">
+        <v>17</v>
+      </c>
+      <c r="Z28">
+        <v>18</v>
+      </c>
+      <c r="AA28">
+        <v>19</v>
+      </c>
+      <c r="AB28">
+        <v>20</v>
+      </c>
+      <c r="AC28">
+        <v>21</v>
+      </c>
+      <c r="AD28">
+        <v>22</v>
+      </c>
+      <c r="AE28">
+        <v>23</v>
+      </c>
+      <c r="AF28">
+        <v>24</v>
+      </c>
+      <c r="AG28">
+        <v>25</v>
+      </c>
+      <c r="AH28">
+        <v>26</v>
+      </c>
+      <c r="AI28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+      <c r="AD30">
+        <v>1</v>
+      </c>
+      <c r="AF30">
+        <v>1</v>
+      </c>
+      <c r="AG30">
+        <v>1</v>
+      </c>
+      <c r="AH30">
+        <v>1</v>
+      </c>
+      <c r="AI30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+      <c r="AD31">
+        <v>1</v>
+      </c>
+      <c r="AF31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="AA32">
+        <v>1</v>
+      </c>
+      <c r="AC32">
+        <v>1</v>
+      </c>
+      <c r="AF32">
+        <v>1</v>
+      </c>
+      <c r="AG32">
+        <v>1</v>
+      </c>
+      <c r="AH32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="AA33">
+        <v>1</v>
+      </c>
+      <c r="AC33">
+        <v>1</v>
+      </c>
+      <c r="AF33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+      <c r="AB34">
+        <v>1</v>
+      </c>
+      <c r="AF34">
+        <v>1</v>
+      </c>
+      <c r="AG34">
+        <v>1</v>
+      </c>
+      <c r="AH34">
+        <v>1</v>
+      </c>
+      <c r="AI34">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add position marking to filter out positions that are already set with '1' or '0'
</commit_message>
<xml_diff>
--- a/solutions/small_nonogram_solver.xlsx
+++ b/solutions/small_nonogram_solver.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H155936\Documents\GitHub\codewars\solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A34441-8A3B-4688-895C-CE0F0A5CA204}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC703EC-F60A-4A84-B806-808F064B5A00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,12 +30,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>2, 1</t>
   </si>
   <si>
     <t>1,1</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AI48"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,20 +536,130 @@
     <col min="28" max="38" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="H1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="11">
+        <v>0</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="11">
+        <v>0</v>
+      </c>
+      <c r="T1">
+        <v>1</v>
+      </c>
+      <c r="U1">
+        <v>0</v>
+      </c>
+      <c r="V1">
+        <v>1</v>
+      </c>
+      <c r="W1">
+        <v>0</v>
+      </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+      <c r="Z1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>18</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -562,8 +675,26 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -583,8 +714,41 @@
         <v>4</v>
       </c>
       <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>0</v>
       </c>
@@ -604,8 +768,26 @@
         <v>8</v>
       </c>
       <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>0</v>
       </c>
@@ -626,7 +808,7 @@
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>0</v>
       </c>
@@ -646,8 +828,23 @@
         <v>8</v>
       </c>
       <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>16</v>
+      </c>
+      <c r="U8">
+        <v>8</v>
+      </c>
+      <c r="V8">
+        <v>4</v>
+      </c>
+      <c r="W8">
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>0</v>
       </c>
@@ -668,7 +865,7 @@
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>0</v>
       </c>
@@ -685,10 +882,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -708,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -728,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -752,7 +949,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>0</v>
       </c>

</xml_diff>